<commit_message>
some stats and data processing
</commit_message>
<xml_diff>
--- a/data/10mRecords/GroupA_MAE.xlsx
+++ b/data/10mRecords/GroupA_MAE.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\석사\석사4차\Masters_Thesis_atINHA\data\10mRecords\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803856C1-B25A-4626-8AC1-24D540D1C68A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9D1624-B48F-43F4-A4CB-B6B02E6E54F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="demographic" sheetId="2" r:id="rId1"/>
-    <sheet name="records" sheetId="1" r:id="rId2"/>
+    <sheet name="records" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -184,18 +183,6 @@
       <t>윤상현</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Height(m)</t>
-  </si>
-  <si>
-    <t>Weight(kg)</t>
   </si>
 </sst>
 </file>
@@ -547,194 +534,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B819D05B-E002-48E8-BD44-6ACBD968FC5E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>26</v>
-      </c>
-      <c r="C2">
-        <v>1.9</v>
-      </c>
-      <c r="D2">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>25</v>
-      </c>
-      <c r="C3">
-        <v>1.7</v>
-      </c>
-      <c r="D3">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>24</v>
-      </c>
-      <c r="D4">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>25</v>
-      </c>
-      <c r="D5">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>26</v>
-      </c>
-      <c r="C6">
-        <v>1.77</v>
-      </c>
-      <c r="D6">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>21</v>
-      </c>
-      <c r="D7">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>22</v>
-      </c>
-      <c r="D8">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
-        <v>23</v>
-      </c>
-      <c r="D9">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10">
-        <v>20</v>
-      </c>
-      <c r="C10">
-        <v>1.69</v>
-      </c>
-      <c r="D10">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11">
-        <v>22</v>
-      </c>
-      <c r="C11">
-        <v>1.86</v>
-      </c>
-      <c r="D11">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12">
-        <v>25</v>
-      </c>
-      <c r="C12">
-        <v>1.75</v>
-      </c>
-      <c r="D12">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13">
-        <v>23</v>
-      </c>
-      <c r="C13">
-        <v>1.77</v>
-      </c>
-      <c r="D13">
-        <v>64</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A2:A13"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>